<commit_message>
extra cost data calculations
</commit_message>
<xml_diff>
--- a/raw/cost_data.xlsx
+++ b/raw/cost_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/AndrewKao/Documents/Grad/G2/QuantEcon/Modeling/wheat/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{58E90B08-ED80-A84D-BF60-EEDD98989A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9340DDA-FA3C-314D-9E13-01095B99DCB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2700" yWindow="2820" windowWidth="26440" windowHeight="15440" xr2:uid="{C69418F5-C978-ED4A-8803-A9CD3D05CA00}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="15">
   <si>
     <t>actual</t>
   </si>
@@ -51,13 +51,43 @@
   </si>
   <si>
     <t>variance</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>crit upper</t>
+  </si>
+  <si>
+    <t>crit lower</t>
+  </si>
+  <si>
+    <t>lower bd</t>
+  </si>
+  <si>
+    <t>upper bd</t>
+  </si>
+  <si>
+    <t>crit</t>
+  </si>
+  <si>
+    <t>std dev</t>
+  </si>
+  <si>
+    <t>mean (log nu)</t>
+  </si>
+  <si>
+    <t>mean (nu)</t>
+  </si>
+  <si>
+    <t>nu^5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -69,6 +99,12 @@
       <sz val="9"/>
       <color theme="1"/>
       <name val="TimesNewRoman"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial Unicode MS"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -91,9 +127,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -408,10 +445,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7D973D1-963C-EC4B-92B6-DC227ED896A6}">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:P16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -642,6 +679,223 @@
         <v>6.6653325957975922E-3</v>
       </c>
     </row>
+    <row r="6" spans="1:16" ht="17">
+      <c r="K6" t="s">
+        <v>6</v>
+      </c>
+      <c r="L6" s="2">
+        <f>_xlfn.CHISQ.INV(1 - 0.025, P6-1)</f>
+        <v>24.735604884931536</v>
+      </c>
+      <c r="M6" t="s">
+        <v>7</v>
+      </c>
+      <c r="N6" s="2">
+        <f>_xlfn.CHISQ.INV( 0.025, P6-1)</f>
+        <v>5.0087505118103319</v>
+      </c>
+      <c r="O6" t="s">
+        <v>5</v>
+      </c>
+      <c r="P6">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16">
+      <c r="K7" t="s">
+        <v>8</v>
+      </c>
+      <c r="L7">
+        <f>(P6-1)*P5/L6</f>
+        <v>3.5030202070438889E-3</v>
+      </c>
+      <c r="M7" t="s">
+        <v>9</v>
+      </c>
+      <c r="N7">
+        <f>(P6-1)*P5/N6</f>
+        <v>1.7299588698030541E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16">
+      <c r="O8" t="s">
+        <v>12</v>
+      </c>
+      <c r="P8">
+        <f>AVERAGE(A4:N4)</f>
+        <v>1.809095473044512E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16">
+      <c r="K9" t="s">
+        <v>10</v>
+      </c>
+      <c r="L9">
+        <f>_xlfn.T.INV.2T(0.025, P6-1)</f>
+        <v>2.5326378146609487</v>
+      </c>
+      <c r="M9" t="s">
+        <v>11</v>
+      </c>
+      <c r="N9">
+        <f>SQRT(P5)</f>
+        <v>8.164148820175679E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16">
+      <c r="K10" t="s">
+        <v>8</v>
+      </c>
+      <c r="L10">
+        <f>P8-(L9*N9/SQRT(P6))</f>
+        <v>-3.7170203331715321E-2</v>
+      </c>
+      <c r="M10" t="s">
+        <v>9</v>
+      </c>
+      <c r="N10">
+        <f>P8+(L9*N9/SQRT(P6))</f>
+        <v>7.3352112792605562E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16">
+      <c r="O11" t="s">
+        <v>13</v>
+      </c>
+      <c r="P11">
+        <f>AVERAGE(G3:N3)</f>
+        <v>1.0034248121737326</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16">
+      <c r="M12" t="s">
+        <v>11</v>
+      </c>
+      <c r="N12">
+        <f>SQRT(P12)</f>
+        <v>8.7341280580494909E-2</v>
+      </c>
+      <c r="O12" t="s">
+        <v>4</v>
+      </c>
+      <c r="P12">
+        <f>VARA(A3:N3)</f>
+        <v>7.6284992934407365E-3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16">
+      <c r="K13" t="s">
+        <v>8</v>
+      </c>
+      <c r="L13">
+        <f>P11-(L9*N12/SQRT(P6))</f>
+        <v>0.94430560185774071</v>
+      </c>
+      <c r="M13" t="s">
+        <v>9</v>
+      </c>
+      <c r="N13">
+        <f>P11+(L9*N12/SQRT(P6))</f>
+        <v>1.0625440224897245</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16">
+      <c r="A14">
+        <f>A3^5</f>
+        <v>1.2518678399818923</v>
+      </c>
+      <c r="B14">
+        <f t="shared" ref="B14:N14" si="2">B3^5</f>
+        <v>0.82485367351957861</v>
+      </c>
+      <c r="C14">
+        <f t="shared" si="2"/>
+        <v>0.76107705587097663</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="2"/>
+        <v>0.97567026617895469</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="2"/>
+        <v>1.3216224883285987</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="2"/>
+        <v>3.2547519629207398</v>
+      </c>
+      <c r="G14">
+        <f t="shared" si="2"/>
+        <v>1.1917902627067594</v>
+      </c>
+      <c r="H14">
+        <f t="shared" si="2"/>
+        <v>1.4261026531991019</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="2"/>
+        <v>0.8092906470434823</v>
+      </c>
+      <c r="J14">
+        <f t="shared" si="2"/>
+        <v>0.97134861404990869</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="2"/>
+        <v>1.3850974191455929</v>
+      </c>
+      <c r="L14">
+        <f t="shared" si="2"/>
+        <v>0.96226853186493266</v>
+      </c>
+      <c r="M14">
+        <f t="shared" si="2"/>
+        <v>0.5618309738749091</v>
+      </c>
+      <c r="N14">
+        <f t="shared" si="2"/>
+        <v>1.0751552142574532</v>
+      </c>
+      <c r="O14" t="s">
+        <v>14</v>
+      </c>
+      <c r="P14">
+        <f>AVERAGE(A14:N14)</f>
+        <v>1.1980519716387772</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16">
+      <c r="M15" t="s">
+        <v>11</v>
+      </c>
+      <c r="N15">
+        <f>SQRT(P15)</f>
+        <v>0.64407925020913148</v>
+      </c>
+      <c r="O15" t="s">
+        <v>4</v>
+      </c>
+      <c r="P15">
+        <f>VARA(A14:N14)</f>
+        <v>0.41483808054995702</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16">
+      <c r="K16" t="s">
+        <v>8</v>
+      </c>
+      <c r="L16">
+        <f>P14-(L9*N15/SQRT(P6))</f>
+        <v>0.76209023166649303</v>
+      </c>
+      <c r="M16" t="s">
+        <v>9</v>
+      </c>
+      <c r="N16">
+        <f>P14+(L9*N15/SQRT(P6))</f>
+        <v>1.6340137116110613</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>